<commit_message>
Corrige los cuadros para 4 nuevos sectores
-Corrige los cuadros usados para la WEB para los sectores estudiados en
la segunda ronda de Informes Sectoriales (Pesca, Minería, etc.)
</commit_message>
<xml_diff>
--- a/data/cuadros/Comercio, Hoteles y Restaurantes/bh.xlsx
+++ b/data/cuadros/Comercio, Hoteles y Restaurantes/bh.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="128">
   <si>
     <t>Participación del empleo del sector en la región</t>
   </si>
@@ -396,12 +396,15 @@
   <si>
     <t xml:space="preserve">20,3 </t>
   </si>
+  <si>
+    <t/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1561">
+  <fonts count="1760">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -6654,8 +6657,809 @@
       <name val="Times New Roman"/>
       <b/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <b/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <b/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <b/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <b/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
-  <fills count="506">
+  <fills count="569">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9182,8 +9986,323 @@
         <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1161">
+  <borders count="1308">
     <border>
       <left/>
       <right/>
@@ -17551,11 +18670,1070 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1161">
+  <cellXfs count="1308">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -22194,6 +24372,594 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="1560" fillId="0" borderId="1160" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1561" fillId="0" borderId="1161" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1562" fillId="0" borderId="1162" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1563" fillId="0" borderId="1163" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1564" fillId="0" borderId="1164" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1565" fillId="0" borderId="1165" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1566" fillId="0" borderId="1166" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1567" fillId="0" borderId="1167" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1568" fillId="0" borderId="1168" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1569" fillId="0" borderId="1169" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1570" fillId="0" borderId="1170" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1571" fillId="0" borderId="1171" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1572" fillId="0" borderId="1172" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1573" fillId="0" borderId="1173" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1574" fillId="0" borderId="1174" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1575" fillId="0" borderId="1175" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1576" fillId="0" borderId="1176" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1577" fillId="0" borderId="1177" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1578" fillId="0" borderId="1178" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1579" fillId="0" borderId="1179" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1580" fillId="0" borderId="1180" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1581" fillId="0" borderId="1181" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1582" fillId="0" borderId="1182" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1583" fillId="0" borderId="1183" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1584" fillId="0" borderId="1184" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1585" fillId="0" borderId="1185" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1586" fillId="0" borderId="1186" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1587" fillId="0" borderId="1187" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1588" fillId="0" borderId="1188" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1589" fillId="0" borderId="1189" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1590" fillId="0" borderId="1190" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1591" fillId="0" borderId="1191" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1592" fillId="0" borderId="1192" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1594" fillId="0" borderId="1193" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1596" fillId="0" borderId="1194" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1598" fillId="0" borderId="1195" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1600" fillId="0" borderId="1196" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1602" fillId="0" borderId="1197" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1604" fillId="0" borderId="1198" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1606" fillId="0" borderId="1199" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1608" fillId="0" borderId="1200" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1610" fillId="0" borderId="1201" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1612" fillId="0" borderId="1202" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1614" fillId="0" borderId="1203" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1616" fillId="0" borderId="1204" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1618" fillId="0" borderId="1205" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1620" fillId="0" borderId="1206" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1622" fillId="0" borderId="1207" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1624" fillId="0" borderId="1208" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1626" fillId="0" borderId="1209" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1628" fillId="0" borderId="1210" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1630" fillId="0" borderId="1211" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1632" fillId="0" borderId="1212" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1634" fillId="0" borderId="1213" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1636" fillId="0" borderId="1214" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1638" fillId="0" borderId="1215" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1640" fillId="0" borderId="1216" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1642" fillId="0" borderId="1217" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1644" fillId="0" borderId="1218" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1646" fillId="0" borderId="1219" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1648" fillId="0" borderId="1220" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1650" fillId="0" borderId="1221" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1652" fillId="0" borderId="1222" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1654" fillId="0" borderId="1223" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1656" fillId="0" borderId="1224" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1658" fillId="0" borderId="1225" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1660" fillId="0" borderId="1226" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1662" fillId="0" borderId="1227" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1664" fillId="0" borderId="1228" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1666" fillId="0" borderId="1229" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1668" fillId="0" borderId="1230" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1670" fillId="0" borderId="1231" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1672" fillId="0" borderId="1232" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1674" fillId="0" borderId="1233" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1676" fillId="0" borderId="1234" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1678" fillId="0" borderId="1235" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1680" fillId="0" borderId="1236" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1682" fillId="0" borderId="1237" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1684" fillId="0" borderId="1238" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1686" fillId="0" borderId="1239" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1688" fillId="0" borderId="1240" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1689" fillId="506" borderId="1241" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1690" fillId="507" borderId="1242" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1691" fillId="508" borderId="1243" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1692" fillId="509" borderId="1244" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1693" fillId="510" borderId="1245" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1694" fillId="511" borderId="1246" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1695" fillId="512" borderId="1247" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1696" fillId="513" borderId="1248" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1697" fillId="514" borderId="1249" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1698" fillId="515" borderId="1250" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1699" fillId="516" borderId="1251" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1700" fillId="517" borderId="1252" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1701" fillId="518" borderId="1253" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1702" fillId="519" borderId="1254" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1703" fillId="520" borderId="1255" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1704" fillId="521" borderId="1256" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1705" fillId="522" borderId="1257" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1706" fillId="523" borderId="1258" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1707" fillId="524" borderId="1259" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1708" fillId="525" borderId="1260" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1709" fillId="526" borderId="1261" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1710" fillId="527" borderId="1262" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1711" fillId="528" borderId="1263" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1712" fillId="529" borderId="1264" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1713" fillId="530" borderId="1265" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1714" fillId="531" borderId="1266" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1715" fillId="532" borderId="1267" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1716" fillId="533" borderId="1268" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1717" fillId="534" borderId="1269" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1718" fillId="535" borderId="1270" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1719" fillId="536" borderId="1271" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1720" fillId="537" borderId="1272" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1721" fillId="538" borderId="1273" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1722" fillId="539" borderId="1274" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1723" fillId="540" borderId="1275" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1724" fillId="541" borderId="1276" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1725" fillId="542" borderId="1277" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1726" fillId="543" borderId="1278" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1727" fillId="544" borderId="1279" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1728" fillId="545" borderId="1280" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1729" fillId="546" borderId="1281" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1730" fillId="547" borderId="1282" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1731" fillId="548" borderId="1283" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1732" fillId="549" borderId="1284" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1733" fillId="550" borderId="1285" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1734" fillId="551" borderId="1286" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1735" fillId="552" borderId="1287" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1736" fillId="553" borderId="1288" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1737" fillId="554" borderId="1289" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1738" fillId="555" borderId="1290" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1739" fillId="556" borderId="1291" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1740" fillId="557" borderId="1292" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1741" fillId="558" borderId="1293" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1742" fillId="559" borderId="1294" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1743" fillId="560" borderId="1295" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1744" fillId="561" borderId="1296" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1745" fillId="562" borderId="1297" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1746" fillId="563" borderId="1298" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1747" fillId="564" borderId="1299" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1748" fillId="565" borderId="1300" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1749" fillId="566" borderId="1301" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1750" fillId="567" borderId="1302" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1751" fillId="568" borderId="1303" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1753" fillId="0" borderId="1304" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1755" fillId="0" borderId="1305" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1757" fillId="0" borderId="1306" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1759" fillId="0" borderId="1307" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -22210,183 +24976,183 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1160" t="s">
+      <c r="A1" s="1307" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1156" t="s">
+      <c r="A2" s="1301" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="1157" t="s">
+      <c r="B2" s="1302" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1158" t="s">
+      <c r="C2" s="1303" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1099" t="s">
+      <c r="A3" s="1244" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1100" t="s">
+      <c r="B3" s="1245" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="1101" t="s">
+      <c r="C3" s="1246" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1102" t="s">
+      <c r="A4" s="1247" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1103" t="s">
+      <c r="B4" s="1248" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="1104" t="s">
+      <c r="C4" s="1249" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1105" t="s">
+      <c r="A5" s="1250" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1106" t="s">
+      <c r="B5" s="1251" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="1107" t="s">
+      <c r="C5" s="1252" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1108" t="s">
+      <c r="A6" s="1253" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1109" t="s">
+      <c r="B6" s="1254" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="1110" t="s">
+      <c r="C6" s="1255" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1111" t="s">
+      <c r="A7" s="1256" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1112" t="s">
+      <c r="B7" s="1257" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="1113" t="s">
+      <c r="C7" s="1258" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1114" t="s">
+      <c r="A8" s="1259" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1115" t="s">
+      <c r="B8" s="1260" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="1116" t="s">
+      <c r="C8" s="1261" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1117" t="s">
+      <c r="A9" s="1262" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1118" t="s">
+      <c r="B9" s="1263" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="1119" t="s">
+      <c r="C9" s="1264" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1120" t="s">
+      <c r="A10" s="1265" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1121" t="s">
+      <c r="B10" s="1266" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="1122" t="s">
+      <c r="C10" s="1267" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1123" t="s">
+      <c r="A11" s="1268" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1124" t="s">
+      <c r="B11" s="1269" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="1125" t="s">
+      <c r="C11" s="1270" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1126" t="s">
+      <c r="A12" s="1271" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1127" t="s">
+      <c r="B12" s="1272" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="1128" t="s">
+      <c r="C12" s="1273" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1129" t="s">
+      <c r="A13" s="1274" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1130" t="s">
+      <c r="B13" s="1275" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="1131" t="s">
+      <c r="C13" s="1276" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1132" t="s">
+      <c r="A14" s="1277" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1133" t="s">
+      <c r="B14" s="1278" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="1134" t="s">
+      <c r="C14" s="1279" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1135" t="s">
+      <c r="A15" s="1280" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1136" t="s">
+      <c r="B15" s="1281" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="1137" t="s">
+      <c r="C15" s="1282" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1150" t="s">
+      <c r="A16" s="1295" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1151" t="s">
+      <c r="B16" s="1296" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="1152" t="s">
+      <c r="C16" s="1297" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1153" t="s">
+      <c r="A17" s="1298" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1154" t="s">
+      <c r="B17" s="1299" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="1155" t="s">
+      <c r="C17" s="1300" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>